<commit_message>
Make Template Download Function
</commit_message>
<xml_diff>
--- a/public/Dataset/raport.xlsx
+++ b/public/Dataset/raport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\File\UNDIP\PKL\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6D4041-C056-4D9F-81E9-DD78162BBD79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ADCAE7C-17F2-4056-AFD8-16B9AD46FACC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{34CDC9F1-779D-4C87-A2AC-F2CA43227A1D}"/>
   </bookViews>
@@ -66,18 +66,6 @@
     <t>Bahasa Jawa</t>
   </si>
   <si>
-    <t>Jurusan1</t>
-  </si>
-  <si>
-    <t>Jurusan2</t>
-  </si>
-  <si>
-    <t>Jurusan3</t>
-  </si>
-  <si>
-    <t>Jurusan4</t>
-  </si>
-  <si>
     <t>Peminatan</t>
   </si>
   <si>
@@ -100,6 +88,18 @@
   </si>
   <si>
     <t>kode</t>
+  </si>
+  <si>
+    <t>MTK GEO</t>
+  </si>
+  <si>
+    <t>BIO SEJ</t>
+  </si>
+  <si>
+    <t>FIS SOS</t>
+  </si>
+  <si>
+    <t>KIM EKO</t>
   </si>
 </sst>
 </file>
@@ -466,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D01C404-435E-4D2D-A4F1-15CF20E0647B}">
   <dimension ref="A1:Q217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
-      <selection activeCell="E209" sqref="E209"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,10 +484,10 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -520,19 +520,19 @@
         <v>10</v>
       </c>
       <c r="M1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" t="s">
         <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -2448,7 +2448,7 @@
         <v>1001</v>
       </c>
       <c r="B38" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C38">
         <v>38</v>
@@ -2501,7 +2501,7 @@
         <v>1002</v>
       </c>
       <c r="B39" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C39">
         <v>31</v>
@@ -2554,7 +2554,7 @@
         <v>1003</v>
       </c>
       <c r="B40" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C40">
         <v>29</v>
@@ -2607,7 +2607,7 @@
         <v>1004</v>
       </c>
       <c r="B41" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C41">
         <v>61</v>
@@ -2660,7 +2660,7 @@
         <v>1005</v>
       </c>
       <c r="B42" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C42">
         <v>99</v>
@@ -2713,7 +2713,7 @@
         <v>1006</v>
       </c>
       <c r="B43" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C43">
         <v>23</v>
@@ -2766,7 +2766,7 @@
         <v>1007</v>
       </c>
       <c r="B44" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C44">
         <v>34</v>
@@ -2819,7 +2819,7 @@
         <v>1008</v>
       </c>
       <c r="B45" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C45">
         <v>52</v>
@@ -2872,7 +2872,7 @@
         <v>1009</v>
       </c>
       <c r="B46" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C46">
         <v>88</v>
@@ -2925,7 +2925,7 @@
         <v>1010</v>
       </c>
       <c r="B47" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C47">
         <v>30</v>
@@ -2978,7 +2978,7 @@
         <v>1011</v>
       </c>
       <c r="B48" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C48">
         <v>22</v>
@@ -3031,7 +3031,7 @@
         <v>1012</v>
       </c>
       <c r="B49" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C49">
         <v>93</v>
@@ -3084,7 +3084,7 @@
         <v>1013</v>
       </c>
       <c r="B50" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C50">
         <v>21</v>
@@ -3137,7 +3137,7 @@
         <v>1014</v>
       </c>
       <c r="B51" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C51">
         <v>70</v>
@@ -3190,7 +3190,7 @@
         <v>1015</v>
       </c>
       <c r="B52" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C52">
         <v>71</v>
@@ -3243,7 +3243,7 @@
         <v>1016</v>
       </c>
       <c r="B53" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C53">
         <v>11</v>
@@ -3296,7 +3296,7 @@
         <v>1017</v>
       </c>
       <c r="B54" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C54">
         <v>14</v>
@@ -3349,7 +3349,7 @@
         <v>1018</v>
       </c>
       <c r="B55" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C55">
         <v>76</v>
@@ -3402,7 +3402,7 @@
         <v>1019</v>
       </c>
       <c r="B56" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C56">
         <v>12</v>
@@ -3455,7 +3455,7 @@
         <v>1020</v>
       </c>
       <c r="B57" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C57">
         <v>35</v>
@@ -3508,7 +3508,7 @@
         <v>1021</v>
       </c>
       <c r="B58" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C58">
         <v>10</v>
@@ -3561,7 +3561,7 @@
         <v>1022</v>
       </c>
       <c r="B59" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C59">
         <v>97</v>
@@ -3614,7 +3614,7 @@
         <v>1023</v>
       </c>
       <c r="B60" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C60">
         <v>33</v>
@@ -3667,7 +3667,7 @@
         <v>1024</v>
       </c>
       <c r="B61" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C61">
         <v>33</v>
@@ -3720,7 +3720,7 @@
         <v>1025</v>
       </c>
       <c r="B62" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C62">
         <v>69</v>
@@ -3773,7 +3773,7 @@
         <v>1026</v>
       </c>
       <c r="B63" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C63">
         <v>12</v>
@@ -3826,7 +3826,7 @@
         <v>1027</v>
       </c>
       <c r="B64" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C64">
         <v>20</v>
@@ -3879,7 +3879,7 @@
         <v>1028</v>
       </c>
       <c r="B65" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C65">
         <v>50</v>
@@ -3932,7 +3932,7 @@
         <v>1029</v>
       </c>
       <c r="B66" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C66">
         <v>97</v>
@@ -3985,7 +3985,7 @@
         <v>1030</v>
       </c>
       <c r="B67" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C67">
         <v>35</v>
@@ -4038,7 +4038,7 @@
         <v>1031</v>
       </c>
       <c r="B68" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C68">
         <v>16</v>
@@ -4091,7 +4091,7 @@
         <v>1032</v>
       </c>
       <c r="B69" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C69">
         <v>38</v>
@@ -4144,7 +4144,7 @@
         <v>1033</v>
       </c>
       <c r="B70" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C70">
         <v>60</v>
@@ -4197,7 +4197,7 @@
         <v>1034</v>
       </c>
       <c r="B71" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C71">
         <v>31</v>
@@ -4250,7 +4250,7 @@
         <v>1035</v>
       </c>
       <c r="B72" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C72">
         <v>96</v>
@@ -4303,7 +4303,7 @@
         <v>1036</v>
       </c>
       <c r="B73" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C73">
         <v>64</v>
@@ -4356,7 +4356,7 @@
         <v>1001</v>
       </c>
       <c r="B74" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C74">
         <v>84</v>
@@ -4409,7 +4409,7 @@
         <v>1002</v>
       </c>
       <c r="B75" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C75">
         <v>50</v>
@@ -4462,7 +4462,7 @@
         <v>1003</v>
       </c>
       <c r="B76" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C76">
         <v>88</v>
@@ -4515,7 +4515,7 @@
         <v>1004</v>
       </c>
       <c r="B77" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C77">
         <v>100</v>
@@ -4568,7 +4568,7 @@
         <v>1005</v>
       </c>
       <c r="B78" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C78">
         <v>19</v>
@@ -4621,7 +4621,7 @@
         <v>1006</v>
       </c>
       <c r="B79" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C79">
         <v>67</v>
@@ -4674,7 +4674,7 @@
         <v>1007</v>
       </c>
       <c r="B80" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C80">
         <v>28</v>
@@ -4727,7 +4727,7 @@
         <v>1008</v>
       </c>
       <c r="B81" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C81">
         <v>74</v>
@@ -4780,7 +4780,7 @@
         <v>1009</v>
       </c>
       <c r="B82" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C82">
         <v>76</v>
@@ -4833,7 +4833,7 @@
         <v>1010</v>
       </c>
       <c r="B83" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C83">
         <v>32</v>
@@ -4886,7 +4886,7 @@
         <v>1011</v>
       </c>
       <c r="B84" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C84">
         <v>93</v>
@@ -4939,7 +4939,7 @@
         <v>1012</v>
       </c>
       <c r="B85" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C85">
         <v>24</v>
@@ -4992,7 +4992,7 @@
         <v>1013</v>
       </c>
       <c r="B86" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C86">
         <v>11</v>
@@ -5045,7 +5045,7 @@
         <v>1014</v>
       </c>
       <c r="B87" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C87">
         <v>56</v>
@@ -5098,7 +5098,7 @@
         <v>1015</v>
       </c>
       <c r="B88" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C88">
         <v>78</v>
@@ -5151,7 +5151,7 @@
         <v>1016</v>
       </c>
       <c r="B89" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C89">
         <v>94</v>
@@ -5204,7 +5204,7 @@
         <v>1017</v>
       </c>
       <c r="B90" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C90">
         <v>59</v>
@@ -5257,7 +5257,7 @@
         <v>1018</v>
       </c>
       <c r="B91" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C91">
         <v>18</v>
@@ -5310,7 +5310,7 @@
         <v>1019</v>
       </c>
       <c r="B92" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C92">
         <v>97</v>
@@ -5363,7 +5363,7 @@
         <v>1020</v>
       </c>
       <c r="B93" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C93">
         <v>58</v>
@@ -5416,7 +5416,7 @@
         <v>1021</v>
       </c>
       <c r="B94" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C94">
         <v>22</v>
@@ -5469,7 +5469,7 @@
         <v>1022</v>
       </c>
       <c r="B95" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C95">
         <v>70</v>
@@ -5522,7 +5522,7 @@
         <v>1023</v>
       </c>
       <c r="B96" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C96">
         <v>75</v>
@@ -5575,7 +5575,7 @@
         <v>1024</v>
       </c>
       <c r="B97" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C97">
         <v>70</v>
@@ -5628,7 +5628,7 @@
         <v>1025</v>
       </c>
       <c r="B98" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C98">
         <v>55</v>
@@ -5681,7 +5681,7 @@
         <v>1026</v>
       </c>
       <c r="B99" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C99">
         <v>28</v>
@@ -5734,7 +5734,7 @@
         <v>1027</v>
       </c>
       <c r="B100" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C100">
         <v>81</v>
@@ -5787,7 +5787,7 @@
         <v>1028</v>
       </c>
       <c r="B101" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C101">
         <v>34</v>
@@ -5840,7 +5840,7 @@
         <v>1029</v>
       </c>
       <c r="B102" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C102">
         <v>94</v>
@@ -5893,7 +5893,7 @@
         <v>1030</v>
       </c>
       <c r="B103" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C103">
         <v>59</v>
@@ -5946,7 +5946,7 @@
         <v>1031</v>
       </c>
       <c r="B104" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C104">
         <v>82</v>
@@ -5999,7 +5999,7 @@
         <v>1032</v>
       </c>
       <c r="B105" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C105">
         <v>71</v>
@@ -6052,7 +6052,7 @@
         <v>1033</v>
       </c>
       <c r="B106" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C106">
         <v>80</v>
@@ -6105,7 +6105,7 @@
         <v>1034</v>
       </c>
       <c r="B107" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C107">
         <v>27</v>
@@ -6158,7 +6158,7 @@
         <v>1035</v>
       </c>
       <c r="B108" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C108">
         <v>42</v>
@@ -6211,7 +6211,7 @@
         <v>1036</v>
       </c>
       <c r="B109" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C109">
         <v>72</v>
@@ -6264,7 +6264,7 @@
         <v>1001</v>
       </c>
       <c r="B110" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C110">
         <v>18</v>
@@ -6317,7 +6317,7 @@
         <v>1002</v>
       </c>
       <c r="B111" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C111">
         <v>22</v>
@@ -6370,7 +6370,7 @@
         <v>1003</v>
       </c>
       <c r="B112" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C112">
         <v>25</v>
@@ -6423,7 +6423,7 @@
         <v>1004</v>
       </c>
       <c r="B113" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C113">
         <v>28</v>
@@ -6476,7 +6476,7 @@
         <v>1005</v>
       </c>
       <c r="B114" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C114">
         <v>31</v>
@@ -6529,7 +6529,7 @@
         <v>1006</v>
       </c>
       <c r="B115" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C115">
         <v>39</v>
@@ -6582,7 +6582,7 @@
         <v>1007</v>
       </c>
       <c r="B116" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C116">
         <v>11</v>
@@ -6635,7 +6635,7 @@
         <v>1008</v>
       </c>
       <c r="B117" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C117">
         <v>21</v>
@@ -6688,7 +6688,7 @@
         <v>1009</v>
       </c>
       <c r="B118" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C118">
         <v>81</v>
@@ -6741,7 +6741,7 @@
         <v>1010</v>
       </c>
       <c r="B119" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C119">
         <v>14</v>
@@ -6794,7 +6794,7 @@
         <v>1011</v>
       </c>
       <c r="B120" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C120">
         <v>89</v>
@@ -6847,7 +6847,7 @@
         <v>1012</v>
       </c>
       <c r="B121" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C121">
         <v>42</v>
@@ -6900,7 +6900,7 @@
         <v>1013</v>
       </c>
       <c r="B122" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C122">
         <v>72</v>
@@ -6953,7 +6953,7 @@
         <v>1014</v>
       </c>
       <c r="B123" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C123">
         <v>67</v>
@@ -7006,7 +7006,7 @@
         <v>1015</v>
       </c>
       <c r="B124" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C124">
         <v>36</v>
@@ -7059,7 +7059,7 @@
         <v>1016</v>
       </c>
       <c r="B125" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C125">
         <v>93</v>
@@ -7112,7 +7112,7 @@
         <v>1017</v>
       </c>
       <c r="B126" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C126">
         <v>69</v>
@@ -7165,7 +7165,7 @@
         <v>1018</v>
       </c>
       <c r="B127" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C127">
         <v>42</v>
@@ -7218,7 +7218,7 @@
         <v>1019</v>
       </c>
       <c r="B128" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C128">
         <v>100</v>
@@ -7271,7 +7271,7 @@
         <v>1020</v>
       </c>
       <c r="B129" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C129">
         <v>32</v>
@@ -7324,7 +7324,7 @@
         <v>1021</v>
       </c>
       <c r="B130" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C130">
         <v>88</v>
@@ -7377,7 +7377,7 @@
         <v>1022</v>
       </c>
       <c r="B131" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C131">
         <v>26</v>
@@ -7430,7 +7430,7 @@
         <v>1023</v>
       </c>
       <c r="B132" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C132">
         <v>58</v>
@@ -7483,7 +7483,7 @@
         <v>1024</v>
       </c>
       <c r="B133" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C133">
         <v>83</v>
@@ -7536,7 +7536,7 @@
         <v>1025</v>
       </c>
       <c r="B134" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C134">
         <v>33</v>
@@ -7589,7 +7589,7 @@
         <v>1026</v>
       </c>
       <c r="B135" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C135">
         <v>54</v>
@@ -7642,7 +7642,7 @@
         <v>1027</v>
       </c>
       <c r="B136" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C136">
         <v>22</v>
@@ -7695,7 +7695,7 @@
         <v>1028</v>
       </c>
       <c r="B137" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C137">
         <v>76</v>
@@ -7748,7 +7748,7 @@
         <v>1029</v>
       </c>
       <c r="B138" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C138">
         <v>38</v>
@@ -7801,7 +7801,7 @@
         <v>1030</v>
       </c>
       <c r="B139" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C139">
         <v>31</v>
@@ -7854,7 +7854,7 @@
         <v>1031</v>
       </c>
       <c r="B140" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C140">
         <v>29</v>
@@ -7907,7 +7907,7 @@
         <v>1032</v>
       </c>
       <c r="B141" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C141">
         <v>61</v>
@@ -7960,7 +7960,7 @@
         <v>1033</v>
       </c>
       <c r="B142" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C142">
         <v>99</v>
@@ -8013,7 +8013,7 @@
         <v>1034</v>
       </c>
       <c r="B143" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C143">
         <v>23</v>
@@ -8066,7 +8066,7 @@
         <v>1035</v>
       </c>
       <c r="B144" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C144">
         <v>34</v>
@@ -8119,7 +8119,7 @@
         <v>1036</v>
       </c>
       <c r="B145" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C145">
         <v>52</v>
@@ -8172,7 +8172,7 @@
         <v>1001</v>
       </c>
       <c r="B146" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C146">
         <v>88</v>
@@ -8225,7 +8225,7 @@
         <v>1002</v>
       </c>
       <c r="B147" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C147">
         <v>30</v>
@@ -8278,7 +8278,7 @@
         <v>1003</v>
       </c>
       <c r="B148" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C148">
         <v>22</v>
@@ -8331,7 +8331,7 @@
         <v>1004</v>
       </c>
       <c r="B149" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C149">
         <v>93</v>
@@ -8384,7 +8384,7 @@
         <v>1005</v>
       </c>
       <c r="B150" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C150">
         <v>21</v>
@@ -8437,7 +8437,7 @@
         <v>1006</v>
       </c>
       <c r="B151" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C151">
         <v>70</v>
@@ -8490,7 +8490,7 @@
         <v>1007</v>
       </c>
       <c r="B152" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C152">
         <v>71</v>
@@ -8543,7 +8543,7 @@
         <v>1008</v>
       </c>
       <c r="B153" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C153">
         <v>11</v>
@@ -8596,7 +8596,7 @@
         <v>1009</v>
       </c>
       <c r="B154" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C154">
         <v>14</v>
@@ -8649,7 +8649,7 @@
         <v>1010</v>
       </c>
       <c r="B155" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C155">
         <v>76</v>
@@ -8702,7 +8702,7 @@
         <v>1011</v>
       </c>
       <c r="B156" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C156">
         <v>12</v>
@@ -8755,7 +8755,7 @@
         <v>1012</v>
       </c>
       <c r="B157" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C157">
         <v>35</v>
@@ -8808,7 +8808,7 @@
         <v>1013</v>
       </c>
       <c r="B158" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C158">
         <v>10</v>
@@ -8861,7 +8861,7 @@
         <v>1014</v>
       </c>
       <c r="B159" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C159">
         <v>97</v>
@@ -8914,7 +8914,7 @@
         <v>1015</v>
       </c>
       <c r="B160" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C160">
         <v>33</v>
@@ -8967,7 +8967,7 @@
         <v>1016</v>
       </c>
       <c r="B161" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C161">
         <v>33</v>
@@ -9020,7 +9020,7 @@
         <v>1017</v>
       </c>
       <c r="B162" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C162">
         <v>69</v>
@@ -9073,7 +9073,7 @@
         <v>1018</v>
       </c>
       <c r="B163" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C163">
         <v>12</v>
@@ -9126,7 +9126,7 @@
         <v>1019</v>
       </c>
       <c r="B164" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C164">
         <v>20</v>
@@ -9179,7 +9179,7 @@
         <v>1020</v>
       </c>
       <c r="B165" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C165">
         <v>50</v>
@@ -9232,7 +9232,7 @@
         <v>1021</v>
       </c>
       <c r="B166" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C166">
         <v>97</v>
@@ -9285,7 +9285,7 @@
         <v>1022</v>
       </c>
       <c r="B167" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C167">
         <v>35</v>
@@ -9338,7 +9338,7 @@
         <v>1023</v>
       </c>
       <c r="B168" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C168">
         <v>16</v>
@@ -9391,7 +9391,7 @@
         <v>1024</v>
       </c>
       <c r="B169" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C169">
         <v>38</v>
@@ -9444,7 +9444,7 @@
         <v>1025</v>
       </c>
       <c r="B170" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C170">
         <v>60</v>
@@ -9497,7 +9497,7 @@
         <v>1026</v>
       </c>
       <c r="B171" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C171">
         <v>31</v>
@@ -9550,7 +9550,7 @@
         <v>1027</v>
       </c>
       <c r="B172" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C172">
         <v>96</v>
@@ -9603,7 +9603,7 @@
         <v>1028</v>
       </c>
       <c r="B173" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C173">
         <v>64</v>
@@ -9656,7 +9656,7 @@
         <v>1029</v>
       </c>
       <c r="B174" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C174">
         <v>84</v>
@@ -9709,7 +9709,7 @@
         <v>1030</v>
       </c>
       <c r="B175" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C175">
         <v>50</v>
@@ -9762,7 +9762,7 @@
         <v>1031</v>
       </c>
       <c r="B176" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C176">
         <v>88</v>
@@ -9815,7 +9815,7 @@
         <v>1032</v>
       </c>
       <c r="B177" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C177">
         <v>100</v>
@@ -9868,7 +9868,7 @@
         <v>1033</v>
       </c>
       <c r="B178" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C178">
         <v>19</v>
@@ -9921,7 +9921,7 @@
         <v>1034</v>
       </c>
       <c r="B179" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C179">
         <v>67</v>
@@ -9974,7 +9974,7 @@
         <v>1035</v>
       </c>
       <c r="B180" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C180">
         <v>28</v>
@@ -10027,7 +10027,7 @@
         <v>1036</v>
       </c>
       <c r="B181" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C181">
         <v>74</v>
@@ -10080,7 +10080,7 @@
         <v>1001</v>
       </c>
       <c r="B182" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C182">
         <v>76</v>
@@ -10133,7 +10133,7 @@
         <v>1002</v>
       </c>
       <c r="B183" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C183">
         <v>32</v>
@@ -10186,7 +10186,7 @@
         <v>1003</v>
       </c>
       <c r="B184" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C184">
         <v>93</v>
@@ -10239,7 +10239,7 @@
         <v>1004</v>
       </c>
       <c r="B185" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C185">
         <v>24</v>
@@ -10292,7 +10292,7 @@
         <v>1005</v>
       </c>
       <c r="B186" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C186">
         <v>11</v>
@@ -10345,7 +10345,7 @@
         <v>1006</v>
       </c>
       <c r="B187" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C187">
         <v>56</v>
@@ -10398,7 +10398,7 @@
         <v>1007</v>
       </c>
       <c r="B188" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C188">
         <v>78</v>
@@ -10451,7 +10451,7 @@
         <v>1008</v>
       </c>
       <c r="B189" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C189">
         <v>94</v>
@@ -10504,7 +10504,7 @@
         <v>1009</v>
       </c>
       <c r="B190" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C190">
         <v>59</v>
@@ -10557,7 +10557,7 @@
         <v>1010</v>
       </c>
       <c r="B191" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C191">
         <v>18</v>
@@ -10610,7 +10610,7 @@
         <v>1011</v>
       </c>
       <c r="B192" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C192">
         <v>97</v>
@@ -10663,7 +10663,7 @@
         <v>1012</v>
       </c>
       <c r="B193" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C193">
         <v>58</v>
@@ -10716,7 +10716,7 @@
         <v>1013</v>
       </c>
       <c r="B194" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C194">
         <v>22</v>
@@ -10769,7 +10769,7 @@
         <v>1014</v>
       </c>
       <c r="B195" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C195">
         <v>70</v>
@@ -10822,7 +10822,7 @@
         <v>1015</v>
       </c>
       <c r="B196" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C196">
         <v>75</v>
@@ -10875,7 +10875,7 @@
         <v>1016</v>
       </c>
       <c r="B197" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C197">
         <v>70</v>
@@ -10928,7 +10928,7 @@
         <v>1017</v>
       </c>
       <c r="B198" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C198">
         <v>55</v>
@@ -10981,7 +10981,7 @@
         <v>1018</v>
       </c>
       <c r="B199" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C199">
         <v>28</v>
@@ -11034,7 +11034,7 @@
         <v>1019</v>
       </c>
       <c r="B200" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C200">
         <v>81</v>
@@ -11087,7 +11087,7 @@
         <v>1020</v>
       </c>
       <c r="B201" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C201">
         <v>34</v>
@@ -11140,7 +11140,7 @@
         <v>1021</v>
       </c>
       <c r="B202" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C202">
         <v>94</v>
@@ -11193,7 +11193,7 @@
         <v>1022</v>
       </c>
       <c r="B203" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C203">
         <v>59</v>
@@ -11246,7 +11246,7 @@
         <v>1023</v>
       </c>
       <c r="B204" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C204">
         <v>82</v>
@@ -11299,7 +11299,7 @@
         <v>1024</v>
       </c>
       <c r="B205" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C205">
         <v>71</v>
@@ -11352,7 +11352,7 @@
         <v>1025</v>
       </c>
       <c r="B206" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C206">
         <v>80</v>
@@ -11405,7 +11405,7 @@
         <v>1026</v>
       </c>
       <c r="B207" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C207">
         <v>27</v>
@@ -11458,7 +11458,7 @@
         <v>1027</v>
       </c>
       <c r="B208" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C208">
         <v>42</v>
@@ -11511,7 +11511,7 @@
         <v>1028</v>
       </c>
       <c r="B209" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C209">
         <v>72</v>
@@ -11564,7 +11564,7 @@
         <v>1029</v>
       </c>
       <c r="B210" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C210">
         <v>18</v>
@@ -11617,7 +11617,7 @@
         <v>1030</v>
       </c>
       <c r="B211" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C211">
         <v>22</v>
@@ -11670,7 +11670,7 @@
         <v>1031</v>
       </c>
       <c r="B212" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C212">
         <v>25</v>
@@ -11723,7 +11723,7 @@
         <v>1032</v>
       </c>
       <c r="B213" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C213">
         <v>28</v>
@@ -11776,7 +11776,7 @@
         <v>1033</v>
       </c>
       <c r="B214" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C214">
         <v>31</v>
@@ -11829,7 +11829,7 @@
         <v>1034</v>
       </c>
       <c r="B215" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C215">
         <v>39</v>
@@ -11882,7 +11882,7 @@
         <v>1035</v>
       </c>
       <c r="B216" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C216">
         <v>11</v>
@@ -11935,7 +11935,7 @@
         <v>1036</v>
       </c>
       <c r="B217" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C217">
         <v>21</v>

</xml_diff>